<commit_message>
Rectified few errors, on excel sheet update and indeed scraper
</commit_message>
<xml_diff>
--- a/sheets/devops.xlsx
+++ b/sheets/devops.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,84 +480,98 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sesamy</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Chief Technology Officer</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Markus Ahlstrand</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>markus@sesamy.com</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Devops</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Estimated $62.1K - $78.6K a year</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Does not have a source link on OpsWorks Co.</t>
-        </is>
+          <t>zoom</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sesamy</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Chief Financial Officer</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Carolina Walther</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>carolina@sesamy.com</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Devops</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Estimated $62.1K - $78.6K a year</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Does not have a source link on OpsWorks Co.</t>
+          <t>zoom</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>nClouds</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CRO</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Scott Jensen</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>scottjensen@nclouds.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>AWS Terraform Kubernetes Ansible Puppet Docker Python Jenkins</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>5 years</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>$124K - $157K</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/rc/clk?jk=c45674b9f68a5d3c&amp;fccid=c76149658a7e6a8d&amp;vjs=3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed version 1 for proxy on indeed
</commit_message>
<xml_diff>
--- a/sheets/devops.xlsx
+++ b/sheets/devops.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,45 +433,51 @@
     <col width="50" customWidth="1" min="6" max="6"/>
     <col width="50" customWidth="1" min="7" max="7"/>
     <col width="50" customWidth="1" min="8" max="8"/>
+    <col width="50" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Company</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Designation</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Responsible Person</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Emails</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Tech stack</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Experience</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Salary</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Source Link</t>
         </is>
@@ -480,98 +486,141 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>zoom</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
+          <t>DevOps Engineer III</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>RELI Group, Inc.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Chief Financial Officer</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Carm Caruso</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>carm.caruso@religroupinc.com</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Python AWS Azure Jenkins Docker Kubernetes Terraform</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>7 years</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/rc/clk?jk=a4bae8a95f641804&amp;fccid=380ad6d2bbbee773&amp;vjs=3</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>zoom</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
+          <t>DevOps Engineer III</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>RELI Group, Inc.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CTO</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Michael Reinhold</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>mike.reinhold@religroupinc.com</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Python AWS Azure Jenkins Docker Kubernetes Terraform</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>7 years</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/rc/clk?jk=a4bae8a95f641804&amp;fccid=380ad6d2bbbee773&amp;vjs=3</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>nClouds</t>
+          <t>DevOps Engineer III</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CRO</t>
+          <t>RELI Group, Inc.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Scott Jensen</t>
+          <t>Talent Acquisition Specialist</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>scottjensen@nclouds.com</t>
+          <t>Denice Cross</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>AWS Terraform Kubernetes Ansible Puppet Docker Python Jenkins</t>
+          <t>denice.cross@religroupinc.com</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>5 years</t>
+          <t>Python AWS Azure Jenkins Docker Kubernetes Terraform</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>$124K - $157K</t>
+          <t>7 years</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://www.indeed.com/rc/clk?jk=c45674b9f68a5d3c&amp;fccid=c76149658a7e6a8d&amp;vjs=3</t>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://www.indeed.com/rc/clk?jk=a4bae8a95f641804&amp;fccid=380ad6d2bbbee773&amp;vjs=3</t>
         </is>
       </c>
     </row>

</xml_diff>